<commit_message>
Changes in css of about added a chatbot screen
</commit_message>
<xml_diff>
--- a/src/faq.xlsx
+++ b/src/faq.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Slim 5\Riddhi\Website\personal-website\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF33A036-9A3B-4D48-9536-4F39796BBC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AADCE9-AC1D-4940-85D9-B4A8AE03CE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{490B6BB1-B403-4ED2-8F5A-98223D853D51}"/>
   </bookViews>
@@ -35,12 +35,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Question</t>
   </si>
   <si>
     <t>Answer</t>
+  </si>
+  <si>
+    <t>what is her name</t>
+  </si>
+  <si>
+    <t>Riddhi Hedaoo</t>
   </si>
 </sst>
 </file>
@@ -401,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B4DBF9-74B5-4A33-B350-C83EE29D7C60}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -417,6 +423,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>